<commit_message>
add new tests for ExcelParser
change interface for IParsers.Parse; add ToxyDocument to implement Word
parser
</commit_message>
<xml_diff>
--- a/Toxy.Test/testdata/Excel/Formatting.xlsx
+++ b/Toxy.Test/testdata/Excel/Formatting.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="15135" windowHeight="8130"/>
@@ -58,21 +58,22 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
-    <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="167" formatCode="yy/mm/dd"/>
-    <numFmt numFmtId="168" formatCode="d/m/yy;@"/>
-    <numFmt numFmtId="169" formatCode="dd\-mm\-yy"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
-    <numFmt numFmtId="172" formatCode="&quot;£&quot;#,##0.00"/>
+  <numFmts count="9">
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="178" formatCode="yy/mm/dd"/>
+    <numFmt numFmtId="179" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="180" formatCode="dd\-mm\-yy"/>
+    <numFmt numFmtId="181" formatCode="0.000"/>
+    <numFmt numFmtId="182" formatCode="0.0"/>
+    <numFmt numFmtId="183" formatCode="&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="185" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -80,8 +81,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -107,19 +115,19 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -127,7 +135,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -414,17 +422,17 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.25" customWidth="1"/>
+    <col min="2" max="2" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -432,7 +440,7 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="10">
         <v>39045</v>
       </c>
     </row>
@@ -440,7 +448,7 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>39045</v>
       </c>
     </row>
@@ -448,7 +456,7 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>39045</v>
       </c>
     </row>
@@ -456,7 +464,7 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>39045</v>
       </c>
     </row>
@@ -464,7 +472,7 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>39045</v>
       </c>
     </row>
@@ -472,15 +480,15 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>39045</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="B8" s="7"/>
+      <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -496,7 +504,7 @@
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7">
         <v>10.52</v>
       </c>
     </row>
@@ -504,7 +512,7 @@
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>10.52</v>
       </c>
     </row>
@@ -512,13 +520,14 @@
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <v>10.52</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -528,8 +537,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -540,8 +550,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>